<commit_message>
added PD-1 example images
</commit_message>
<xml_diff>
--- a/metadata/annotation_task.xlsx
+++ b/metadata/annotation_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/amir_livne_intel_com/Documents/Desktop/PDL1-predictor_annotator/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_7F75F5B6872052B4163DAFB2415ED87656CD9988" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{739FF855-6022-48E3-9C62-40E2BE62106D}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_7F75F5B6872052B4163DAFB2415ED87656CD9988" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{42EE20A4-0D2B-441C-994F-37397C985AE5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>HE_path</t>
   </si>
@@ -95,6 +95,36 @@
   </si>
   <si>
     <t>\PDL1(SP142)-Springbio\PDL1(SP142)-Springbio_A12_v3_b3_009.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_000.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_001.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_002.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_003.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_004.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_005.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_006.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_007.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_008.jpg</t>
+  </si>
+  <si>
+    <t>\PD1(NAT105)-CellMarque\PD1(NAT105)-CellMarque_A12_v3_b3_009.jpg</t>
   </si>
 </sst>
 </file>
@@ -460,7 +490,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,24 +498,24 @@
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="1"/>
@@ -497,6 +527,9 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -505,6 +538,9 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -513,6 +549,9 @@
       <c r="B4" t="s">
         <v>10</v>
       </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -521,6 +560,9 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -529,6 +571,9 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -537,6 +582,9 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -545,6 +593,9 @@
       <c r="B8" t="s">
         <v>18</v>
       </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -553,6 +604,9 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -561,6 +615,9 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -568,6 +625,9 @@
       </c>
       <c r="B11" t="s">
         <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>